<commit_message>
api onboarding and check module file
</commit_message>
<xml_diff>
--- a/project_details.xlsx
+++ b/project_details.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="plant" sheetId="3" r:id="rId1"/>
-    <sheet name="asset" sheetId="2" r:id="rId2"/>
+    <sheet name="demo" sheetId="4" r:id="rId2"/>
+    <sheet name="asset" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
   <si>
     <t>50MW BHILAI</t>
   </si>
@@ -498,6 +499,12 @@
   </si>
   <si>
     <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>data_freq</t>
+  </si>
+  <si>
+    <t>Demo Project</t>
   </si>
 </sst>
 </file>
@@ -905,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,7 +962,9 @@
       <c r="J1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="K1" s="5"/>
+      <c r="K1" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -985,6 +994,9 @@
       <c r="J2" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -1011,6 +1023,9 @@
       <c r="J3" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="K3" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -1037,6 +1052,9 @@
       <c r="J4" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="K4" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -1063,6 +1081,9 @@
       <c r="J5" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -1088,6 +1109,9 @@
       </c>
       <c r="J6" s="1" t="s">
         <v>142</v>
+      </c>
+      <c r="K6" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1115,6 +1139,9 @@
       <c r="J7" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="K7" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -1141,6 +1168,9 @@
       <c r="J8" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="K8" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -1167,6 +1197,9 @@
       <c r="J9" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="K9" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1193,6 +1226,9 @@
       <c r="J10" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="K10" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -1219,6 +1255,9 @@
       <c r="J11" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="K11" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -1245,6 +1284,9 @@
       <c r="J12" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="K12" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -1271,6 +1313,9 @@
       <c r="J13" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="K13" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -1297,6 +1342,9 @@
       <c r="J14" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="K14" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -1323,6 +1371,9 @@
       <c r="J15" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="K15" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -1349,8 +1400,11 @@
       <c r="J16" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1375,8 +1429,11 @@
       <c r="J17" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1401,8 +1458,11 @@
       <c r="J18" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1427,8 +1487,11 @@
       <c r="J19" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1453,8 +1516,11 @@
       <c r="J20" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1479,8 +1545,11 @@
       <c r="J21" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1505,8 +1574,11 @@
       <c r="J22" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1531,8 +1603,11 @@
       <c r="J23" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1557,8 +1632,11 @@
       <c r="J24" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1583,8 +1661,11 @@
       <c r="J25" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1609,8 +1690,11 @@
       <c r="J26" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1635,8 +1719,11 @@
       <c r="J27" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1661,8 +1748,11 @@
       <c r="J28" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1687,8 +1777,11 @@
       <c r="J29" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1713,8 +1806,11 @@
       <c r="J30" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1739,8 +1835,11 @@
       <c r="J31" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1765,8 +1864,11 @@
       <c r="J32" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1791,8 +1893,11 @@
       <c r="J33" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K33" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1817,8 +1922,11 @@
       <c r="J34" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1843,8 +1951,11 @@
       <c r="J35" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1869,8 +1980,11 @@
       <c r="J36" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K36" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1895,8 +2009,11 @@
       <c r="J37" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K37" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1921,8 +2038,11 @@
       <c r="J38" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K38" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1947,8 +2067,11 @@
       <c r="J39" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K39" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1973,8 +2096,11 @@
       <c r="J40" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K40" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1999,8 +2125,11 @@
       <c r="J41" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K41" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2025,8 +2154,11 @@
       <c r="J42" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K42" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2051,8 +2183,11 @@
       <c r="J43" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K43" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2077,8 +2212,11 @@
       <c r="J44" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K44" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2103,8 +2241,11 @@
       <c r="J45" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K45" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2129,8 +2270,11 @@
       <c r="J46" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K46" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2155,8 +2299,11 @@
       <c r="J47" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K47" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2181,8 +2328,11 @@
       <c r="J48" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K48" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2207,8 +2357,11 @@
       <c r="J49" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K49" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2233,8 +2386,11 @@
       <c r="J50" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K50" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2259,8 +2415,11 @@
       <c r="J51" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K51" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2285,8 +2444,11 @@
       <c r="J52" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K52" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2311,8 +2473,11 @@
       <c r="J53" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K53" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2337,8 +2502,11 @@
       <c r="J54" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K54" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2363,8 +2531,11 @@
       <c r="J55" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K55" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2389,8 +2560,11 @@
       <c r="J56" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K56" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2415,8 +2589,11 @@
       <c r="J57" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K57" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2441,8 +2618,11 @@
       <c r="J58" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K58" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2467,8 +2647,11 @@
       <c r="J59" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K59" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2493,8 +2676,11 @@
       <c r="J60" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K60" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2519,8 +2705,11 @@
       <c r="J61" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K61" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2545,8 +2734,11 @@
       <c r="J62" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K62" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2571,8 +2763,11 @@
       <c r="J63" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K63" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2597,8 +2792,11 @@
       <c r="J64" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K64" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2623,8 +2821,11 @@
       <c r="J65" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K65" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2649,8 +2850,11 @@
       <c r="J66" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K66" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2675,8 +2879,11 @@
       <c r="J67" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K67" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2701,8 +2908,11 @@
       <c r="J68" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K68" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2727,8 +2937,11 @@
       <c r="J69" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K69" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2753,8 +2966,11 @@
       <c r="J70" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K70" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2779,8 +2995,11 @@
       <c r="J71" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K71" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2805,8 +3024,11 @@
       <c r="J72" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K72" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2831,8 +3053,11 @@
       <c r="J73" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K73" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -2857,8 +3082,11 @@
       <c r="J74" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K74" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -2883,8 +3111,11 @@
       <c r="J75" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K75" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -2909,8 +3140,11 @@
       <c r="J76" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K76" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -2935,8 +3169,11 @@
       <c r="J77" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K77" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -2961,8 +3198,11 @@
       <c r="J78" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K78" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -2987,8 +3227,11 @@
       <c r="J79" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K79" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3013,8 +3256,11 @@
       <c r="J80" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K80" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3039,8 +3285,11 @@
       <c r="J81" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K81" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3065,8 +3314,11 @@
       <c r="J82" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K82" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3091,8 +3343,11 @@
       <c r="J83" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K83" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3117,8 +3372,11 @@
       <c r="J84" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K84" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3143,8 +3401,11 @@
       <c r="J85" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K85" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -3169,8 +3430,11 @@
       <c r="J86" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K86" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -3195,8 +3459,11 @@
       <c r="J87" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K87" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -3221,8 +3488,11 @@
       <c r="J88" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K88" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -3247,8 +3517,11 @@
       <c r="J89" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K89" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -3273,8 +3546,11 @@
       <c r="J90" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K90" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -3299,13 +3575,136 @@
       <c r="J91" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
+      <c r="K91" s="1">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>81.471800000000002</v>
+      </c>
+      <c r="G2" s="1">
+        <v>21.235299999999999</v>
+      </c>
+      <c r="H2" s="1">
+        <v>75571</v>
+      </c>
+      <c r="I2" s="1">
+        <v>50050</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>76.980900000000005</v>
+      </c>
+      <c r="G3" s="1">
+        <v>29.317299999999999</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3075</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2560</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Modification in api onboarding file
</commit_message>
<xml_diff>
--- a/project_details.xlsx
+++ b/project_details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="164">
   <si>
     <t>50MW BHILAI</t>
   </si>
@@ -504,7 +504,10 @@
     <t>data_freq</t>
   </si>
   <si>
-    <t>Demo Project</t>
+    <t>Demo Project 01</t>
+  </si>
+  <si>
+    <t>Demo Project 02</t>
   </si>
 </sst>
 </file>
@@ -3590,7 +3593,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3676,7 +3679,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>

</xml_diff>